<commit_message>
main changes to get instruction id
main:
changes would identify what instruction are passed
</commit_message>
<xml_diff>
--- a/Book1 (version 1).xlsx
+++ b/Book1 (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakim\Documents\GitHub\ECE-5367-Un-Pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A594F6-FC7D-4FFE-9E5C-01DE709BF887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873F5EE9-2EBA-4A05-BD51-994BEC37C1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29BFCFB4-3CD1-41F9-B711-FDA20C2A0A6A}"/>
+    <workbookView xWindow="7392" yWindow="5112" windowWidth="17280" windowHeight="8964" xr2:uid="{29BFCFB4-3CD1-41F9-B711-FDA20C2A0A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>add</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>FunCodeBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -351,6 +354,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -360,9 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,25 +680,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD78506A-4569-46E8-8A1F-F6938467EFD7}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="9.44140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="11" customWidth="1"/>
     <col min="7" max="7" width="9.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="14"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,7 +715,7 @@
       <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -723,12 +727,12 @@
       <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -738,14 +742,14 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>HEX2DEC(C2)</f>
+        <f t="shared" ref="D2:D32" si="0">HEX2DEC(C2)</f>
         <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>HEX2BIN(C2)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G2" s="4">
@@ -759,12 +763,12 @@
         <f>HEX2BIN(G2)</f>
         <v>100000</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="11">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -772,33 +776,33 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>HEX2DEC(C3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E32" si="0">HEX2BIN(C3)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="14" t="s">
+        <f t="shared" ref="E3:E32" si="1">HEX2BIN(C3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="4">
         <v>21</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H13" si="1">HEX2DEC(G3)</f>
+        <f t="shared" ref="H3:H13" si="2">HEX2DEC(G3)</f>
         <v>33</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I13" si="2">HEX2BIN(G3)</f>
+        <f t="shared" ref="I3:I13" si="3">HEX2BIN(G3)</f>
         <v>100001</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -806,33 +810,33 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>HEX2DEC(C4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G4" s="4">
         <v>24</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100100</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -840,33 +844,36 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>HEX2DEC(C5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -874,33 +881,33 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>HEX2DEC(C6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G6" s="4">
         <v>27</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100111</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -908,33 +915,33 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>HEX2DEC(C7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G7" s="4">
         <v>25</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100101</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -942,33 +949,33 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>HEX2DEC(C8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101010</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -976,33 +983,33 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>HEX2DEC(C9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101011</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -1010,33 +1017,33 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>HEX2DEC(C10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1044,33 +1051,33 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>HEX2DEC(C11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -1078,33 +1085,33 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>HEX2DEC(C12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G12" s="4">
         <v>22</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100010</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:12" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
       <c r="B13" s="9" t="s">
         <v>20</v>
       </c>
@@ -1112,33 +1119,33 @@
         <v>0</v>
       </c>
       <c r="D13" s="9">
-        <f>HEX2DEC(C13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="14" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="8">
         <v>3</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1148,19 +1155,19 @@
         <v>8</v>
       </c>
       <c r="D14">
-        <f>HEX2DEC(C14)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1168,19 +1175,19 @@
         <v>9</v>
       </c>
       <c r="D15">
-        <f>HEX2DEC(C15)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1001</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1188,19 +1195,19 @@
         <v>42</v>
       </c>
       <c r="D16">
-        <f>HEX2DEC(C16)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1208,19 +1215,20 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <f>HEX2DEC(C17)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1228,19 +1236,19 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <f>HEX2DEC(C18)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1248,19 +1256,19 @@
         <v>24</v>
       </c>
       <c r="D19">
-        <f>HEX2DEC(C19)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100100</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
       <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1268,19 +1276,19 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <f>HEX2DEC(C20)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100101</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1288,19 +1296,19 @@
         <v>30</v>
       </c>
       <c r="D21">
-        <f>HEX2DEC(C21)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110000</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1308,19 +1316,19 @@
         <v>43</v>
       </c>
       <c r="D22">
-        <f>HEX2DEC(C22)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1328,19 +1336,19 @@
         <v>23</v>
       </c>
       <c r="D23">
-        <f>HEX2DEC(C23)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100011</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1348,19 +1356,19 @@
         <v>44</v>
       </c>
       <c r="D24">
-        <f>HEX2DEC(C24)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1101</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1368,19 +1376,19 @@
         <v>45</v>
       </c>
       <c r="D25">
-        <f>HEX2DEC(C25)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E25" t="str">
         <f>HEX2BIN(C25)</f>
         <v>1010</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1388,19 +1396,19 @@
         <v>46</v>
       </c>
       <c r="D26">
-        <f>HEX2DEC(C26)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1011</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
       <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
@@ -1408,19 +1416,19 @@
         <v>28</v>
       </c>
       <c r="D27">
-        <f>HEX2DEC(C27)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>101000</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
       <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1428,19 +1436,19 @@
         <v>38</v>
       </c>
       <c r="D28">
-        <f>HEX2DEC(C28)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111000</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
       <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
@@ -1448,19 +1456,19 @@
         <v>29</v>
       </c>
       <c r="D29">
-        <f>HEX2DEC(C29)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>101001</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
+    <row r="30" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14"/>
       <c r="B30" s="7" t="s">
         <v>38</v>
       </c>
@@ -1468,20 +1476,20 @@
         <v>47</v>
       </c>
       <c r="D30" s="9">
-        <f>HEX2DEC(C30)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>101011</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1491,19 +1499,19 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <f>HEX2DEC(C31)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
+    <row r="32" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14"/>
       <c r="B32" s="9" t="s">
         <v>41</v>
       </c>
@@ -1511,17 +1519,17 @@
         <v>3</v>
       </c>
       <c r="D32" s="9">
-        <f>HEX2DEC(C32)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J32" s="15"/>
+      <c r="J32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>